<commit_message>
Added more locations and sql executed commands
</commit_message>
<xml_diff>
--- a/locations.xlsx
+++ b/locations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://utpac-my.sharepoint.com/personal/lucia_liu_utp_ac_pa/Documents/Proyectos-Articulos/Tesis/code/TwitterTraffic-Pty/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="279" documentId="8_{36EE6C1E-A6BB-4D3F-909E-92210784B037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{801F8296-DD6D-4C3C-A8C8-CDEC08DB9786}"/>
+  <xr:revisionPtr revIDLastSave="283" documentId="8_{36EE6C1E-A6BB-4D3F-909E-92210784B037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{989BF1FA-6542-442F-A959-F66D7DB78F75}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{260091BF-4F1D-4A09-B579-CAE9649117FA}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="143">
   <si>
     <t>place</t>
   </si>
@@ -104,9 +104,6 @@
     <t>Vía Centenario</t>
   </si>
   <si>
-    <t>Burunga Vía Centenario</t>
-  </si>
-  <si>
     <t>direcci[oó]n (a|hacia) burunga</t>
   </si>
   <si>
@@ -114,9 +111,6 @@
   </si>
   <si>
     <t>Vía Interamericana</t>
-  </si>
-  <si>
-    <t>Burunga Vía Interamericana</t>
   </si>
   <si>
     <t>carretera panamericana burunga panama</t>
@@ -857,9 +851,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F1B844-7F28-4C07-B7A6-39B3E37A6E94}">
   <dimension ref="A1:L206"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H38" sqref="H38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -878,19 +872,19 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>2</v>
@@ -916,7 +910,7 @@
     </row>
     <row r="2" spans="1:12" ht="42" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
@@ -925,7 +919,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>7</v>
@@ -940,7 +934,7 @@
         <v>8</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="K2" s="4" t="str">
         <f>LEFT(J2,SEARCH(",",J2)-1)</f>
@@ -954,7 +948,7 @@
     <row r="3" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>11</v>
@@ -963,7 +957,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>12</v>
@@ -978,7 +972,7 @@
         <v>16</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="K3" s="4" t="str">
         <f t="shared" ref="K3:K12" si="0">LEFT(J3,SEARCH(",",J3)-1)</f>
@@ -992,19 +986,19 @@
     <row r="4" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" ref="A4:A67" si="2">A3+1</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>21</v>
@@ -1016,10 +1010,10 @@
         <v>20</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="K4" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1033,19 +1027,19 @@
     <row r="5" spans="1:12" ht="42" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>21</v>
@@ -1054,13 +1048,13 @@
         <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K5" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1074,31 +1068,31 @@
     <row r="6" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="J6" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="K6" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1112,28 +1106,28 @@
     <row r="7" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E7" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="J7" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="K7" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1147,31 +1141,31 @@
     <row r="8" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="H8" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="K8" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1185,31 +1179,31 @@
     <row r="9" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="H9" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="K9" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1223,31 +1217,31 @@
     <row r="10" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="H10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K10" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1261,31 +1255,31 @@
     <row r="11" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" s="2">
         <v>99</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="H11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="K11" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1299,31 +1293,31 @@
     <row r="12" spans="1:12" ht="42" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="H12" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K12" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1337,1639 +1331,1807 @@
     <row r="13" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="J13" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="K13" s="4" t="str">
+        <f t="shared" ref="K13:K33" si="3">LEFT(J13,SEARCH(",",J13)-1)</f>
+        <v>9.02875</v>
+      </c>
+      <c r="L13" s="4" t="str">
+        <f t="shared" ref="L13:L33" si="4">RIGHT(J13,LEN(J13)-SEARCH(",",J13))</f>
+        <v>-79.51934</v>
       </c>
     </row>
     <row r="14" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="H14" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="K14" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>9.02875</v>
+      </c>
+      <c r="L14" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.51934</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="E15" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F15" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="G15" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
+      </c>
+      <c r="K15" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>9.06885</v>
+      </c>
+      <c r="L15" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.40644</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K16" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>9.02046</v>
+      </c>
+      <c r="L16" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.53090</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
       <c r="B17" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>22</v>
       </c>
       <c r="F17" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="K17" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>9.02646</v>
+      </c>
+      <c r="L17" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.52924</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="K18" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>9.03126</v>
+      </c>
+      <c r="L18" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.51640</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" s="2" t="s">
+      <c r="D19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K19" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>8.9960</v>
+      </c>
+      <c r="L19" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.5314</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="C20" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <f t="shared" si="2"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="H20" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K20" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>8.9918</v>
+      </c>
+      <c r="L20" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.5308</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="J21" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="2" t="s">
+      <c r="K21" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>8.99542</v>
+      </c>
+      <c r="L21" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.53353</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K22" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>9.00942</v>
+      </c>
+      <c r="L22" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.53429</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="42" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <f t="shared" si="2"/>
-        <v>19</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="C23" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K23" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>9.03133</v>
+      </c>
+      <c r="L23" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.50872</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="42" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <f t="shared" si="2"/>
-        <v>21</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="J24" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K24" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>9.03133</v>
+      </c>
+      <c r="L24" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.50872</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="G25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="H22" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="42" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <f t="shared" si="2"/>
-        <v>22</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="J25" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K25" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>8.96739</v>
+      </c>
+      <c r="L25" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.53963</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="55.8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <f t="shared" si="2"/>
-        <v>23</v>
-      </c>
-      <c r="B24" s="2" t="s">
+      <c r="J26" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="K26" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>9.09995</v>
+      </c>
+      <c r="L26" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.38872</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J24" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <f t="shared" si="2"/>
-        <v>24</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="55.8" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <f t="shared" si="2"/>
+      <c r="D27" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="2" t="s">
+      <c r="E27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="F27" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J27" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="K27" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>8.91554</v>
+      </c>
+      <c r="L27" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.74251</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A28">
+      <c r="G28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="K28" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>9.04260</v>
+      </c>
+      <c r="L28" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.41768</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="E28" s="2" t="s">
+      <c r="D29" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G28" s="2" t="s">
+      <c r="F29" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="K29" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>9.0363</v>
+      </c>
+      <c r="L29" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.4256</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="69.599999999999994" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="K30" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>8.99658</v>
+      </c>
+      <c r="L30" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.53711</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="K31" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>8.9905</v>
+      </c>
+      <c r="L31" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.5444</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="K32" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>8.9812</v>
+      </c>
+      <c r="L32" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.5450</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="H28" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="J28" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <f t="shared" si="2"/>
-        <v>28</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="69.599999999999994" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <f t="shared" si="2"/>
+      <c r="B33" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E30" s="2" t="s">
+      <c r="I33" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="K33" s="4" t="str">
+        <f t="shared" si="3"/>
+        <v>8.9746</v>
+      </c>
+      <c r="L33" s="4" t="str">
+        <f t="shared" si="4"/>
+        <v>-79.5540</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F30" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I32" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="28.2" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="C33" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="J33" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A34">
+      <c r="E34" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A35">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35">
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A37">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A38">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A40">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A42">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A42">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A44">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A45">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A45">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A46">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A46">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A47">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A47">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48">
         <f t="shared" si="2"/>
         <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A48">
-        <f t="shared" si="2"/>
-        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50">
         <f t="shared" si="2"/>
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="2"/>
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="2"/>
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="2"/>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="2"/>
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57">
         <f t="shared" si="2"/>
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="2"/>
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="2"/>
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="2"/>
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61">
         <f t="shared" si="2"/>
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" si="2"/>
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="2"/>
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64">
         <f t="shared" si="2"/>
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="2"/>
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="2"/>
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" si="2"/>
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68">
-        <f t="shared" ref="A68:A131" si="3">A67+1</f>
-        <v>67</v>
+        <f t="shared" ref="A68:A131" si="5">A67+1</f>
+        <v>66</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69">
-        <f t="shared" si="3"/>
-        <v>68</v>
+        <f t="shared" si="5"/>
+        <v>67</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70">
-        <f t="shared" si="3"/>
-        <v>69</v>
+        <f t="shared" si="5"/>
+        <v>68</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71">
-        <f t="shared" si="3"/>
-        <v>70</v>
+        <f t="shared" si="5"/>
+        <v>69</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72">
-        <f t="shared" si="3"/>
-        <v>71</v>
+        <f t="shared" si="5"/>
+        <v>70</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73">
-        <f t="shared" si="3"/>
-        <v>72</v>
+        <f t="shared" si="5"/>
+        <v>71</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74">
-        <f t="shared" si="3"/>
-        <v>73</v>
+        <f t="shared" si="5"/>
+        <v>72</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75">
-        <f t="shared" si="3"/>
-        <v>74</v>
+        <f t="shared" si="5"/>
+        <v>73</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76">
-        <f t="shared" si="3"/>
-        <v>75</v>
+        <f t="shared" si="5"/>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77">
-        <f t="shared" si="3"/>
-        <v>76</v>
+        <f t="shared" si="5"/>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78">
-        <f t="shared" si="3"/>
-        <v>77</v>
+        <f t="shared" si="5"/>
+        <v>76</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79">
-        <f t="shared" si="3"/>
-        <v>78</v>
+        <f t="shared" si="5"/>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80">
-        <f t="shared" si="3"/>
-        <v>79</v>
+        <f t="shared" si="5"/>
+        <v>78</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81">
-        <f t="shared" si="3"/>
-        <v>80</v>
+        <f t="shared" si="5"/>
+        <v>79</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82">
-        <f t="shared" si="3"/>
-        <v>81</v>
+        <f t="shared" si="5"/>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A83">
-        <f t="shared" si="3"/>
-        <v>82</v>
+        <f t="shared" si="5"/>
+        <v>81</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A84">
-        <f t="shared" si="3"/>
-        <v>83</v>
+        <f t="shared" si="5"/>
+        <v>82</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A85">
-        <f t="shared" si="3"/>
-        <v>84</v>
+        <f t="shared" si="5"/>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A86">
-        <f t="shared" si="3"/>
-        <v>85</v>
+        <f t="shared" si="5"/>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A87">
-        <f t="shared" si="3"/>
-        <v>86</v>
+        <f t="shared" si="5"/>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A88">
-        <f t="shared" si="3"/>
-        <v>87</v>
+        <f t="shared" si="5"/>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A89">
-        <f t="shared" si="3"/>
-        <v>88</v>
+        <f t="shared" si="5"/>
+        <v>87</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A90">
-        <f t="shared" si="3"/>
-        <v>89</v>
+        <f t="shared" si="5"/>
+        <v>88</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A91">
-        <f t="shared" si="3"/>
-        <v>90</v>
+        <f t="shared" si="5"/>
+        <v>89</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A92">
-        <f t="shared" si="3"/>
-        <v>91</v>
+        <f t="shared" si="5"/>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A93">
-        <f t="shared" si="3"/>
-        <v>92</v>
+        <f t="shared" si="5"/>
+        <v>91</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A94">
-        <f t="shared" si="3"/>
-        <v>93</v>
+        <f t="shared" si="5"/>
+        <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A95">
-        <f t="shared" si="3"/>
-        <v>94</v>
+        <f t="shared" si="5"/>
+        <v>93</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A96">
-        <f t="shared" si="3"/>
-        <v>95</v>
+        <f t="shared" si="5"/>
+        <v>94</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A97">
-        <f t="shared" si="3"/>
-        <v>96</v>
+        <f t="shared" si="5"/>
+        <v>95</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A98">
-        <f t="shared" si="3"/>
-        <v>97</v>
+        <f t="shared" si="5"/>
+        <v>96</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A99">
-        <f t="shared" si="3"/>
-        <v>98</v>
+        <f t="shared" si="5"/>
+        <v>97</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A100">
-        <f t="shared" si="3"/>
-        <v>99</v>
+        <f t="shared" si="5"/>
+        <v>98</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A101">
-        <f t="shared" si="3"/>
-        <v>100</v>
+        <f t="shared" si="5"/>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A102">
-        <f t="shared" si="3"/>
-        <v>101</v>
+        <f t="shared" si="5"/>
+        <v>100</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A103">
-        <f t="shared" si="3"/>
-        <v>102</v>
+        <f t="shared" si="5"/>
+        <v>101</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A104">
-        <f t="shared" si="3"/>
-        <v>103</v>
+        <f t="shared" si="5"/>
+        <v>102</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A105">
-        <f t="shared" si="3"/>
-        <v>104</v>
+        <f t="shared" si="5"/>
+        <v>103</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A106">
-        <f t="shared" si="3"/>
-        <v>105</v>
+        <f t="shared" si="5"/>
+        <v>104</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A107">
-        <f t="shared" si="3"/>
-        <v>106</v>
+        <f t="shared" si="5"/>
+        <v>105</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A108">
-        <f t="shared" si="3"/>
-        <v>107</v>
+        <f t="shared" si="5"/>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A109">
-        <f t="shared" si="3"/>
-        <v>108</v>
+        <f t="shared" si="5"/>
+        <v>107</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A110">
-        <f t="shared" si="3"/>
-        <v>109</v>
+        <f t="shared" si="5"/>
+        <v>108</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A111">
-        <f t="shared" si="3"/>
-        <v>110</v>
+        <f t="shared" si="5"/>
+        <v>109</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A112">
-        <f t="shared" si="3"/>
-        <v>111</v>
+        <f t="shared" si="5"/>
+        <v>110</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A113">
-        <f t="shared" si="3"/>
-        <v>112</v>
+        <f t="shared" si="5"/>
+        <v>111</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A114">
-        <f t="shared" si="3"/>
-        <v>113</v>
+        <f t="shared" si="5"/>
+        <v>112</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A115">
-        <f t="shared" si="3"/>
-        <v>114</v>
+        <f t="shared" si="5"/>
+        <v>113</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A116">
-        <f t="shared" si="3"/>
-        <v>115</v>
+        <f t="shared" si="5"/>
+        <v>114</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A117">
-        <f t="shared" si="3"/>
-        <v>116</v>
+        <f t="shared" si="5"/>
+        <v>115</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A118">
-        <f t="shared" si="3"/>
-        <v>117</v>
+        <f t="shared" si="5"/>
+        <v>116</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A119">
-        <f t="shared" si="3"/>
-        <v>118</v>
+        <f t="shared" si="5"/>
+        <v>117</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A120">
-        <f t="shared" si="3"/>
-        <v>119</v>
+        <f t="shared" si="5"/>
+        <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A121">
-        <f t="shared" si="3"/>
-        <v>120</v>
+        <f t="shared" si="5"/>
+        <v>119</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A122">
-        <f t="shared" si="3"/>
-        <v>121</v>
+        <f t="shared" si="5"/>
+        <v>120</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A123">
-        <f t="shared" si="3"/>
-        <v>122</v>
+        <f t="shared" si="5"/>
+        <v>121</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A124">
-        <f t="shared" si="3"/>
-        <v>123</v>
+        <f t="shared" si="5"/>
+        <v>122</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A125">
-        <f t="shared" si="3"/>
-        <v>124</v>
+        <f t="shared" si="5"/>
+        <v>123</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A126">
-        <f t="shared" si="3"/>
-        <v>125</v>
+        <f t="shared" si="5"/>
+        <v>124</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A127">
-        <f t="shared" si="3"/>
-        <v>126</v>
+        <f t="shared" si="5"/>
+        <v>125</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A128">
-        <f t="shared" si="3"/>
-        <v>127</v>
+        <f t="shared" si="5"/>
+        <v>126</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A129">
-        <f t="shared" si="3"/>
-        <v>128</v>
+        <f t="shared" si="5"/>
+        <v>127</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A130">
-        <f t="shared" si="3"/>
-        <v>129</v>
+        <f t="shared" si="5"/>
+        <v>128</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A131">
-        <f t="shared" si="3"/>
-        <v>130</v>
+        <f t="shared" si="5"/>
+        <v>129</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A132">
-        <f t="shared" ref="A132:A195" si="4">A131+1</f>
-        <v>131</v>
+        <f t="shared" ref="A132:A195" si="6">A131+1</f>
+        <v>130</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A133">
-        <f t="shared" si="4"/>
-        <v>132</v>
+        <f t="shared" si="6"/>
+        <v>131</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A134">
-        <f t="shared" si="4"/>
-        <v>133</v>
+        <f t="shared" si="6"/>
+        <v>132</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A135">
-        <f t="shared" si="4"/>
-        <v>134</v>
+        <f t="shared" si="6"/>
+        <v>133</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A136">
-        <f t="shared" si="4"/>
-        <v>135</v>
+        <f t="shared" si="6"/>
+        <v>134</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A137">
-        <f t="shared" si="4"/>
-        <v>136</v>
+        <f t="shared" si="6"/>
+        <v>135</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A138">
-        <f t="shared" si="4"/>
-        <v>137</v>
+        <f t="shared" si="6"/>
+        <v>136</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A139">
-        <f t="shared" si="4"/>
-        <v>138</v>
+        <f t="shared" si="6"/>
+        <v>137</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A140">
-        <f t="shared" si="4"/>
-        <v>139</v>
+        <f t="shared" si="6"/>
+        <v>138</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A141">
-        <f t="shared" si="4"/>
-        <v>140</v>
+        <f t="shared" si="6"/>
+        <v>139</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A142">
-        <f t="shared" si="4"/>
-        <v>141</v>
+        <f t="shared" si="6"/>
+        <v>140</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A143">
-        <f t="shared" si="4"/>
-        <v>142</v>
+        <f t="shared" si="6"/>
+        <v>141</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A144">
-        <f t="shared" si="4"/>
-        <v>143</v>
+        <f t="shared" si="6"/>
+        <v>142</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A145">
-        <f t="shared" si="4"/>
-        <v>144</v>
+        <f t="shared" si="6"/>
+        <v>143</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A146">
-        <f t="shared" si="4"/>
-        <v>145</v>
+        <f t="shared" si="6"/>
+        <v>144</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A147">
-        <f t="shared" si="4"/>
-        <v>146</v>
+        <f t="shared" si="6"/>
+        <v>145</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A148">
-        <f t="shared" si="4"/>
-        <v>147</v>
+        <f t="shared" si="6"/>
+        <v>146</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A149">
-        <f t="shared" si="4"/>
-        <v>148</v>
+        <f t="shared" si="6"/>
+        <v>147</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A150">
-        <f t="shared" si="4"/>
-        <v>149</v>
+        <f t="shared" si="6"/>
+        <v>148</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A151">
-        <f t="shared" si="4"/>
-        <v>150</v>
+        <f t="shared" si="6"/>
+        <v>149</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A152">
-        <f t="shared" si="4"/>
-        <v>151</v>
+        <f t="shared" si="6"/>
+        <v>150</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A153">
-        <f t="shared" si="4"/>
-        <v>152</v>
+        <f t="shared" si="6"/>
+        <v>151</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A154">
-        <f t="shared" si="4"/>
-        <v>153</v>
+        <f t="shared" si="6"/>
+        <v>152</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A155">
-        <f t="shared" si="4"/>
-        <v>154</v>
+        <f t="shared" si="6"/>
+        <v>153</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A156">
-        <f t="shared" si="4"/>
-        <v>155</v>
+        <f t="shared" si="6"/>
+        <v>154</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A157">
-        <f t="shared" si="4"/>
-        <v>156</v>
+        <f t="shared" si="6"/>
+        <v>155</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A158">
-        <f t="shared" si="4"/>
-        <v>157</v>
+        <f t="shared" si="6"/>
+        <v>156</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A159">
-        <f t="shared" si="4"/>
-        <v>158</v>
+        <f t="shared" si="6"/>
+        <v>157</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A160">
-        <f t="shared" si="4"/>
-        <v>159</v>
+        <f t="shared" si="6"/>
+        <v>158</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A161">
-        <f t="shared" si="4"/>
-        <v>160</v>
+        <f t="shared" si="6"/>
+        <v>159</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A162">
-        <f t="shared" si="4"/>
-        <v>161</v>
+        <f t="shared" si="6"/>
+        <v>160</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A163">
-        <f t="shared" si="4"/>
-        <v>162</v>
+        <f t="shared" si="6"/>
+        <v>161</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A164">
-        <f t="shared" si="4"/>
-        <v>163</v>
+        <f t="shared" si="6"/>
+        <v>162</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A165">
-        <f t="shared" si="4"/>
-        <v>164</v>
+        <f t="shared" si="6"/>
+        <v>163</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A166">
-        <f t="shared" si="4"/>
-        <v>165</v>
+        <f t="shared" si="6"/>
+        <v>164</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A167">
-        <f t="shared" si="4"/>
-        <v>166</v>
+        <f t="shared" si="6"/>
+        <v>165</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A168">
-        <f t="shared" si="4"/>
-        <v>167</v>
+        <f t="shared" si="6"/>
+        <v>166</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A169">
-        <f t="shared" si="4"/>
-        <v>168</v>
+        <f t="shared" si="6"/>
+        <v>167</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A170">
-        <f t="shared" si="4"/>
-        <v>169</v>
+        <f t="shared" si="6"/>
+        <v>168</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A171">
-        <f t="shared" si="4"/>
-        <v>170</v>
+        <f t="shared" si="6"/>
+        <v>169</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A172">
-        <f t="shared" si="4"/>
-        <v>171</v>
+        <f t="shared" si="6"/>
+        <v>170</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A173">
-        <f t="shared" si="4"/>
-        <v>172</v>
+        <f t="shared" si="6"/>
+        <v>171</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A174">
-        <f t="shared" si="4"/>
-        <v>173</v>
+        <f t="shared" si="6"/>
+        <v>172</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A175">
-        <f t="shared" si="4"/>
-        <v>174</v>
+        <f t="shared" si="6"/>
+        <v>173</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A176">
-        <f t="shared" si="4"/>
-        <v>175</v>
+        <f t="shared" si="6"/>
+        <v>174</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A177">
-        <f t="shared" si="4"/>
-        <v>176</v>
+        <f t="shared" si="6"/>
+        <v>175</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A178">
-        <f t="shared" si="4"/>
-        <v>177</v>
+        <f t="shared" si="6"/>
+        <v>176</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A179">
-        <f t="shared" si="4"/>
-        <v>178</v>
+        <f t="shared" si="6"/>
+        <v>177</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A180">
-        <f t="shared" si="4"/>
-        <v>179</v>
+        <f t="shared" si="6"/>
+        <v>178</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A181">
-        <f t="shared" si="4"/>
-        <v>180</v>
+        <f t="shared" si="6"/>
+        <v>179</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A182">
-        <f t="shared" si="4"/>
-        <v>181</v>
+        <f t="shared" si="6"/>
+        <v>180</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A183">
-        <f t="shared" si="4"/>
-        <v>182</v>
+        <f t="shared" si="6"/>
+        <v>181</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A184">
-        <f t="shared" si="4"/>
-        <v>183</v>
+        <f t="shared" si="6"/>
+        <v>182</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A185">
-        <f t="shared" si="4"/>
-        <v>184</v>
+        <f t="shared" si="6"/>
+        <v>183</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A186">
-        <f t="shared" si="4"/>
-        <v>185</v>
+        <f t="shared" si="6"/>
+        <v>184</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A187">
-        <f t="shared" si="4"/>
-        <v>186</v>
+        <f t="shared" si="6"/>
+        <v>185</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A188">
-        <f t="shared" si="4"/>
-        <v>187</v>
+        <f t="shared" si="6"/>
+        <v>186</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A189">
-        <f t="shared" si="4"/>
-        <v>188</v>
+        <f t="shared" si="6"/>
+        <v>187</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A190">
-        <f t="shared" si="4"/>
-        <v>189</v>
+        <f t="shared" si="6"/>
+        <v>188</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A191">
-        <f t="shared" si="4"/>
-        <v>190</v>
+        <f t="shared" si="6"/>
+        <v>189</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A192">
-        <f t="shared" si="4"/>
-        <v>191</v>
+        <f t="shared" si="6"/>
+        <v>190</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A193">
-        <f t="shared" si="4"/>
-        <v>192</v>
+        <f t="shared" si="6"/>
+        <v>191</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A194">
-        <f t="shared" si="4"/>
-        <v>193</v>
+        <f t="shared" si="6"/>
+        <v>192</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A195">
-        <f t="shared" si="4"/>
-        <v>194</v>
+        <f t="shared" si="6"/>
+        <v>193</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A196">
-        <f t="shared" ref="A196:A206" si="5">A195+1</f>
-        <v>195</v>
+        <f t="shared" ref="A196:A206" si="7">A195+1</f>
+        <v>194</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A197">
-        <f t="shared" si="5"/>
-        <v>196</v>
+        <f t="shared" si="7"/>
+        <v>195</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A198">
-        <f t="shared" si="5"/>
-        <v>197</v>
+        <f t="shared" si="7"/>
+        <v>196</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A199">
-        <f t="shared" si="5"/>
-        <v>198</v>
+        <f t="shared" si="7"/>
+        <v>197</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A200">
-        <f t="shared" si="5"/>
-        <v>199</v>
+        <f t="shared" si="7"/>
+        <v>198</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A201">
-        <f t="shared" si="5"/>
-        <v>200</v>
+        <f t="shared" si="7"/>
+        <v>199</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A202">
-        <f t="shared" si="5"/>
-        <v>201</v>
+        <f t="shared" si="7"/>
+        <v>200</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A203">
-        <f t="shared" si="5"/>
-        <v>202</v>
+        <f t="shared" si="7"/>
+        <v>201</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A204">
-        <f t="shared" si="5"/>
-        <v>203</v>
+        <f t="shared" si="7"/>
+        <v>202</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A205">
-        <f t="shared" si="5"/>
-        <v>204</v>
+        <f t="shared" si="7"/>
+        <v>203</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A206">
-        <f t="shared" si="5"/>
-        <v>205</v>
+        <f t="shared" si="7"/>
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Geocoding updates until now
</commit_message>
<xml_diff>
--- a/locations.xlsx
+++ b/locations.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="283" documentId="8_{36EE6C1E-A6BB-4D3F-909E-92210784B037}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{989BF1FA-6542-442F-A959-F66D7DB78F75}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{260091BF-4F1D-4A09-B579-CAE9649117FA}"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13290" xr2:uid="{260091BF-4F1D-4A09-B579-CAE9649117FA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -851,9 +851,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18F1B844-7F28-4C07-B7A6-39B3E37A6E94}">
   <dimension ref="A1:L206"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>